<commit_message>
Fixed search function, cleaned up notes function, make notes perm
</commit_message>
<xml_diff>
--- a/MI_CoverSheets.xlsx
+++ b/MI_CoverSheets.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MI Cover Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9358" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="8059" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -3173,7 +3173,7 @@
     <row r="2" ht="19.5" customHeight="1" s="73">
       <c r="A2" s="79" t="inlineStr">
         <is>
-          <t>9358</t>
+          <t>8059</t>
         </is>
       </c>
       <c r="D2" s="80" t="n"/>
@@ -3196,7 +3196,11 @@
           <t>SAMPLES DUE (Y/N):</t>
         </is>
       </c>
-      <c r="F3" s="86" t="n"/>
+      <c r="F3" s="86" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="G3" s="72" t="n"/>
       <c r="H3" s="87" t="n"/>
       <c r="I3" s="88" t="n"/>
@@ -3235,7 +3239,7 @@
       <c r="B5" s="96" t="n"/>
       <c r="C5" s="97" t="inlineStr">
         <is>
-          <t>06-29-2020</t>
+          <t>01-06-2020</t>
         </is>
       </c>
       <c r="D5" s="75" t="n"/>
@@ -3244,7 +3248,11 @@
           <t>LUBE DUE (Y/N):</t>
         </is>
       </c>
-      <c r="F5" s="93" t="n"/>
+      <c r="F5" s="93" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="G5" s="72" t="n"/>
       <c r="H5" s="94" t="n"/>
       <c r="O5" s="72" t="n"/>
@@ -3255,14 +3263,22 @@
           <t>MI DUE (month):</t>
         </is>
       </c>
-      <c r="C6" s="98" t="n"/>
+      <c r="C6" s="98" t="inlineStr">
+        <is>
+          <t>6mo</t>
+        </is>
+      </c>
       <c r="D6" s="99" t="n"/>
       <c r="E6" s="85" t="inlineStr">
         <is>
           <t>C/S DUE (Y/N):</t>
         </is>
       </c>
-      <c r="F6" s="93" t="n"/>
+      <c r="F6" s="93" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="H6" s="100" t="n"/>
       <c r="K6" s="88" t="n"/>
       <c r="L6" s="88" t="n"/>
@@ -3283,7 +3299,11 @@
           <t>AF DUE (Y/N):</t>
         </is>
       </c>
-      <c r="F7" s="93" t="n"/>
+      <c r="F7" s="93" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
       <c r="H7" s="100" t="n"/>
       <c r="I7" s="89" t="n"/>
       <c r="K7" s="88" t="n"/>
@@ -3642,7 +3662,7 @@
       </c>
       <c r="B24" s="135" t="inlineStr">
         <is>
-          <t>lubbe</t>
+          <t>AIR BRAKE</t>
         </is>
       </c>
       <c r="C24" s="110" t="n"/>
@@ -3660,7 +3680,7 @@
       <c r="A25" s="136" t="n"/>
       <c r="B25" s="137" t="inlineStr">
         <is>
-          <t>it up boyee</t>
+          <t>Alertor penalty, source still present</t>
         </is>
       </c>
       <c r="D25" s="138" t="n"/>

</xml_diff>

<commit_message>
Revisions, cleaned up code
</commit_message>
<xml_diff>
--- a/MI_CoverSheets.xlsx
+++ b/MI_CoverSheets.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MI Cover Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="8059" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4000" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -3173,7 +3173,7 @@
     <row r="2" ht="19.5" customHeight="1" s="73">
       <c r="A2" s="79" t="inlineStr">
         <is>
-          <t>8059</t>
+          <t>4000</t>
         </is>
       </c>
       <c r="D2" s="80" t="n"/>
@@ -3239,7 +3239,7 @@
       <c r="B5" s="96" t="n"/>
       <c r="C5" s="97" t="inlineStr">
         <is>
-          <t>01-06-2020</t>
+          <t>01-17-2020</t>
         </is>
       </c>
       <c r="D5" s="75" t="n"/>
@@ -3248,11 +3248,7 @@
           <t>LUBE DUE (Y/N):</t>
         </is>
       </c>
-      <c r="F5" s="93" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="F5" s="93" t="n"/>
       <c r="G5" s="72" t="n"/>
       <c r="H5" s="94" t="n"/>
       <c r="O5" s="72" t="n"/>
@@ -3662,7 +3658,7 @@
       </c>
       <c r="B24" s="135" t="inlineStr">
         <is>
-          <t>AIR BRAKE</t>
+          <t>PTC TROUBLE</t>
         </is>
       </c>
       <c r="C24" s="110" t="n"/>
@@ -3678,11 +3674,7 @@
     </row>
     <row r="25" ht="19.5" customHeight="1" s="73">
       <c r="A25" s="136" t="n"/>
-      <c r="B25" s="137" t="inlineStr">
-        <is>
-          <t>Alertor penalty, source still present</t>
-        </is>
-      </c>
+      <c r="B25" s="137" t="n"/>
       <c r="D25" s="138" t="n"/>
       <c r="E25" s="139" t="n"/>
       <c r="G25" s="138" t="n"/>

</xml_diff>